<commit_message>
Tarefa 1 e 2 completas
</commit_message>
<xml_diff>
--- a/resultado_comissoes.xlsx
+++ b/resultado_comissoes.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Comissão" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,7 +459,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total a Pagar ao vendedor</t>
+          <t>Comissão Final</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>32</v>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>256</v>
+        <v>320</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>64</v>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>100</v>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>30</v>

</xml_diff>